<commit_message>
Accepted and Rejected papers, making brief notes on each
</commit_message>
<xml_diff>
--- a/3. Literature Review/READ AND REJECTED PAPERS.xlsx
+++ b/3. Literature Review/READ AND REJECTED PAPERS.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonmclain/Documents/Documents/Software Development with AI/Semister 4/Engineering Team Project/TUS-Engineering-Team-Project/3. Literature Review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5350C87-270A-F744-B4AE-29D560E46FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CBE947-43D6-3340-86EC-65204A55E65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{D765FF18-E40D-1C42-96D0-B8F810559842}"/>
+    <workbookView xWindow="32520" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{D765FF18-E40D-1C42-96D0-B8F810559842}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Read  and Rejected list" sheetId="1" r:id="rId1"/>
+    <sheet name="Potential Papers" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,10 +34,194 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+  <si>
+    <t>Forecasting of Covid-19 Using Time Series Regression Models</t>
+  </si>
+  <si>
+    <t>Name of Paper</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Evaluates several models used for time series analsis and selects the best performing, works at a Global level. Discusses several aspects of feature engineering</t>
+  </si>
+  <si>
+    <t>A Predictive Model for Confirmed Cases of COVID-19 in Nigeria</t>
+  </si>
+  <si>
+    <t>A Deep Learning technology based covid-19
+prediction</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>Detection based on X-Rays. Unlikely we can get access to this data source</t>
+  </si>
+  <si>
+    <t>A Review of the Machine Learning Algorithms for Covid-19 Case Analysis</t>
+  </si>
+  <si>
+    <t>Rambling, not very coherent. Not worth reading</t>
+  </si>
+  <si>
+    <t>An Ensemble Machine Learning Approach
+For Time Series Forecasting of COVID-19 Cases</t>
+  </si>
+  <si>
+    <t>Outlines the Ensemble approach and concludes it improves timeseries predictions</t>
+  </si>
+  <si>
+    <t>Analyzing COVID-19 Data using Various Algorithms</t>
+  </si>
+  <si>
+    <t>A good discussion paper for application of ML to predict covid-19</t>
+  </si>
+  <si>
+    <t>Core topic</t>
+  </si>
+  <si>
+    <t>Time series</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Ensemble and Time Series</t>
+  </si>
+  <si>
+    <t>Comparison of LR/ LDR/ KNN/ CART</t>
+  </si>
+  <si>
+    <t>Analysis and Prediction of COVID-19 Pandemic in Bangladesh by using ANFIS and LSTM Network</t>
+  </si>
+  <si>
+    <t>Prediction using ANFIS and LSTM</t>
+  </si>
+  <si>
+    <t>Comparative Study based on Analysis of coronavirus Disease (COVID-19 Detect and Prediciton using Machine Learning Models</t>
+  </si>
+  <si>
+    <t>General discussion paper, good for background but not a lot of depth</t>
+  </si>
+  <si>
+    <t>Classification/ Regression/ Neural Networks</t>
+  </si>
+  <si>
+    <t>COVID-19 Infection Detection Using Machine Learning</t>
+  </si>
+  <si>
+    <t>Discusses prediction based on biometrics, including data from wearables</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>Effect of increased number of COVID-19 tests using supervosed machine learning models</t>
+  </si>
+  <si>
+    <t>Considers the impact when number of testes for COVId-19 equals population of south korea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decision Tree/ Random Forest/ Gaussian Process regression </t>
+  </si>
+  <si>
+    <t>Forecasting COVID19 outbrak throuhg fuson of internest search, social meia and air quality data</t>
+  </si>
+  <si>
+    <t>Novel approach that looks into geospatial predictions based on non-medical data</t>
+  </si>
+  <si>
+    <t>Novel predicition methods</t>
+  </si>
+  <si>
+    <t>Forecasting of COVID19 per regions using ARIMA models and
+polynomial functions</t>
+  </si>
+  <si>
+    <t>Time series with ARIMA</t>
+  </si>
+  <si>
+    <t>Dataset: our world in data</t>
+  </si>
+  <si>
+    <t>Comparing Social media and
+Google to detect and predict severe
+epidemics</t>
+  </si>
+  <si>
+    <t>Social Media data sources. Uses ARIMA</t>
+  </si>
+  <si>
+    <t>Generic to epidemics, useful should we decide to encorporate social media information into our dataset</t>
+  </si>
+  <si>
+    <t>MATHEMATICAL MODELS FOR COVID-19 PANDEMIC: A COMPARATIVE
+ANALYSIS</t>
+  </si>
+  <si>
+    <t>Too complicated for me</t>
+  </si>
+  <si>
+    <t>Pandemic-Aware Day-Ahead Demand
+Forecasting using Ensemble Learning</t>
+  </si>
+  <si>
+    <t>specifically looks into electicity demand forecasting</t>
+  </si>
+  <si>
+    <t>Prediction of the COVID-19 epidemic trends based on SEIR and AI models</t>
+  </si>
+  <si>
+    <t>Proposes a suspected-exposed-infectious-removed model for predicitons in china</t>
+  </si>
+  <si>
+    <t>SEIR</t>
+  </si>
+  <si>
+    <t>Prediction of the COVID-19 pandemic with Machine Learning Models</t>
+  </si>
+  <si>
+    <t>Linear Regression, Lasso, Exponential Smoothing</t>
+  </si>
+  <si>
+    <t>Identifies exponential smoothing as the best performing model for their dataset</t>
+  </si>
+  <si>
+    <t>The study of the effect of the data collected during
+vaccination period on the prediction of the number
+of Covid-19 cases</t>
+  </si>
+  <si>
+    <t>Seems to outline a good idea to consider vaccination rates in models, they prove prediciton results are different during vaccinated and unvaccinated periods. Covers Canada, Germany, UAE and USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linear Regression </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -64,8 +249,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,12 +571,307 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532D31DD-40E7-E246-A156-F56023F42EA5}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="65" customWidth="1"/>
+    <col min="3" max="3" width="84.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA04C650-531C-F04F-BEDD-FED6114FC738}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="77.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Worked on literature review and collecting relevant papers
</commit_message>
<xml_diff>
--- a/3. Literature Review/READ AND REJECTED PAPERS.xlsx
+++ b/3. Literature Review/READ AND REJECTED PAPERS.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonmclain/Documents/Documents/Software Development with AI/Semister 4/Engineering Team Project/TUS-Engineering-Team-Project/3. Literature Review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CBE947-43D6-3340-86EC-65204A55E65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A46693-0025-BC4A-9CA9-38959E31C2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32520" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{D765FF18-E40D-1C42-96D0-B8F810559842}"/>
+    <workbookView xWindow="1400" yWindow="1520" windowWidth="28040" windowHeight="16940" xr2:uid="{D765FF18-E40D-1C42-96D0-B8F810559842}"/>
   </bookViews>
   <sheets>
     <sheet name="Read  and Rejected list" sheetId="1" r:id="rId1"/>
     <sheet name="Potential Papers" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Read  and Rejected list'!$A$1:$D$18</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -571,10 +574,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532D31DD-40E7-E246-A156-F56023F42EA5}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,7 +616,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -626,7 +630,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -766,7 +770,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -780,7 +784,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -849,6 +853,13 @@
       <c r="D20" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D18" xr:uid="{532D31DD-40E7-E246-A156-F56023F42EA5}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Accepted"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>